<commit_message>
- Execution of missing experiments for retures and resolution selection - Not required files deleted
</commit_message>
<xml_diff>
--- a/Accuracy Results_v2.xlsx
+++ b/Accuracy Results_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andree/Dropbox/My Mac (Macbooks-MacBook-Pro.local)/Desktop/occupacny_detection/experimentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F9B26F-EE22-F846-A682-ECC6DDE10065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3737FF8-0115-F046-B582-E15F812BB245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{48E0AA12-B65A-DE4A-8794-21F6F44F596D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{48E0AA12-B65A-DE4A-8794-21F6F44F596D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Selection" sheetId="5" r:id="rId1"/>
@@ -122,8 +122,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -299,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,6 +402,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,15 +436,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,8 +769,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView zoomScale="139" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,36 +783,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="40"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="41"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
       <c r="L2" s="8"/>
       <c r="M2" s="6"/>
     </row>
@@ -1002,37 +1032,37 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="40"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="41"/>
       <c r="G10" s="41"/>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1087,19 +1117,19 @@
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="32">
+      <c r="H12" s="58">
         <v>0.95120000000000005</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="76">
         <v>1</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="59">
         <v>0.99509999999999998</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="78">
         <v>1</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="11">
         <f>AVERAGE(H12:K12)</f>
         <v>0.98657499999999998</v>
       </c>
@@ -1108,36 +1138,36 @@
       <c r="A13" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="51">
         <v>0.78680000000000005</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="52">
         <v>0.92310000000000003</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="52">
         <v>0.91720000000000002</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="53">
         <v>0.98480000000000001</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="54">
         <f>AVERAGE(B13:E13)</f>
         <v>0.90297500000000008</v>
       </c>
       <c r="G13" s="42"/>
-      <c r="H13" s="21">
+      <c r="H13" s="61">
         <v>0.95120000000000005</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="77">
         <v>1</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="39">
         <v>0.98529999999999995</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="79">
         <v>1</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="11">
         <f>AVERAGE(H13:K13)</f>
         <v>0.98412500000000003</v>
       </c>
@@ -1146,79 +1176,83 @@
       <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="55">
         <v>0.94410000000000005</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="56">
         <v>0.95620000000000005</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="56">
         <v>0.95860000000000001</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="57">
         <v>0.96630000000000005</v>
       </c>
-      <c r="F14" s="49">
+      <c r="F14" s="54">
         <f>AVERAGE(B14:E14)</f>
         <v>0.95630000000000004</v>
       </c>
       <c r="G14" s="42"/>
-      <c r="H14" s="25">
+      <c r="H14" s="63">
         <v>0.99509999999999998</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="56">
         <v>0.99509999999999998</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="56">
         <v>0.99019999999999997</v>
       </c>
-      <c r="K14" s="36">
+      <c r="K14" s="80">
         <v>1</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="11">
         <f>AVERAGE(H14:K14)</f>
         <v>0.99509999999999998</v>
+      </c>
+      <c r="M14" s="82">
+        <f>L14-L13</f>
+        <v>1.0974999999999957E-2</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="11">
         <f>AVERAGE(B12:B14)</f>
         <v>0.86545000000000005</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="11">
         <f t="shared" ref="C15:K15" si="2">AVERAGE(C12:C14)</f>
         <v>0.9396500000000001</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="11">
         <f t="shared" si="2"/>
         <v>0.93789999999999996</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="11">
         <f t="shared" si="2"/>
         <v>0.97555000000000003</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8">
+      <c r="H15" s="11">
         <f t="shared" si="2"/>
         <v>0.96583333333333332</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="11">
         <f t="shared" si="2"/>
         <v>0.99836666666666662</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="11">
         <f t="shared" si="2"/>
         <v>0.99020000000000008</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="81">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
@@ -1798,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE825F32-9C12-0943-B876-9338338088B0}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,10 +1846,10 @@
     <col min="12" max="12" width="7.33203125" customWidth="1"/>
     <col min="14" max="17" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.33203125" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -1824,61 +1858,61 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="N3" s="55" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="N3" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55"/>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="55"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+      <c r="U3" s="75"/>
+      <c r="V3" s="75"/>
     </row>
     <row r="4" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
       <c r="G4" s="47"/>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="N4" s="56" t="s">
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="N4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
       <c r="R4" s="47"/>
-      <c r="S4" s="57" t="s">
+      <c r="S4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="74"/>
     </row>
     <row r="5" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
@@ -2220,61 +2254,61 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="N13" s="55" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="N13" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="55"/>
+      <c r="O13" s="75"/>
+      <c r="P13" s="75"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="75"/>
+      <c r="V13" s="75"/>
     </row>
     <row r="14" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="47"/>
-      <c r="H14" s="57" t="s">
+      <c r="H14" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="N14" s="56" t="s">
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="N14" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="73"/>
       <c r="R14" s="47"/>
-      <c r="S14" s="57" t="s">
+      <c r="S14" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="57"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="74"/>
+      <c r="V14" s="74"/>
     </row>
     <row r="15" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -2339,63 +2373,63 @@
       <c r="A16" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="61">
         <v>0.97160000000000002</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="39">
         <v>0.96519999999999995</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="39">
         <v>0.95169999999999999</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="62">
         <v>0.90539999999999998</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="64">
         <f>AVERAGE(B16:E16)</f>
         <v>0.94847499999999996</v>
       </c>
       <c r="G16" s="45"/>
-      <c r="H16" s="21">
+      <c r="H16" s="61">
         <v>0.97560000000000002</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="52">
         <v>0.9657</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="52">
         <v>0.9657</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="53">
         <v>0.89549999999999996</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="11">
         <f>AVERAGE(H16:K16)</f>
         <v>0.95062500000000005</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="58">
         <v>0.99509999999999998</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="59">
         <v>1</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="67">
         <v>1</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="Q16" s="11">
         <f>AVERAGE(N16:P16)</f>
         <v>0.99836666666666662</v>
       </c>
       <c r="R16" s="8"/>
-      <c r="S16" s="32">
+      <c r="S16" s="58">
         <v>1</v>
       </c>
-      <c r="T16" s="37">
+      <c r="T16" s="68">
         <v>0.98570000000000002</v>
       </c>
-      <c r="U16" s="38">
+      <c r="U16" s="60">
         <v>1</v>
       </c>
-      <c r="V16" s="8">
+      <c r="V16" s="11">
         <f>AVERAGE(S16:U16)</f>
         <v>0.9952333333333333</v>
       </c>
@@ -2404,63 +2438,63 @@
       <c r="A17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="51">
         <v>0.98480000000000001</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="52">
         <v>0.97529999999999994</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="52">
         <v>0.9577</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="53">
         <v>0.91039999999999999</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="64">
         <f t="shared" ref="F17:F18" si="5">AVERAGE(B17:E17)</f>
         <v>0.95704999999999996</v>
       </c>
       <c r="G17" s="45"/>
-      <c r="H17" s="23">
+      <c r="H17" s="51">
         <v>0.98819999999999997</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="52">
         <v>0.9768</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="52">
         <v>0.9607</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="53">
         <v>0.94520000000000004</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="11">
         <f>AVERAGE(H17:K17)</f>
         <v>0.96772499999999995</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="51">
         <v>0.99509999999999998</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17" s="52">
         <v>1</v>
       </c>
-      <c r="P17" s="24">
+      <c r="P17" s="53">
         <v>1</v>
       </c>
-      <c r="Q17" s="8">
+      <c r="Q17" s="11">
         <f t="shared" ref="Q17:Q18" si="6">AVERAGE(N17:P17)</f>
         <v>0.99836666666666662</v>
       </c>
       <c r="R17" s="8"/>
-      <c r="S17" s="23">
+      <c r="S17" s="51">
         <v>1</v>
       </c>
-      <c r="T17" s="17">
+      <c r="T17" s="52">
         <v>1</v>
       </c>
-      <c r="U17" s="24">
+      <c r="U17" s="53">
         <v>1</v>
       </c>
-      <c r="V17" s="8">
+      <c r="V17" s="11">
         <f t="shared" ref="V17:V18" si="7">AVERAGE(S17:U17)</f>
         <v>1</v>
       </c>
@@ -2469,63 +2503,63 @@
       <c r="A18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="63">
         <v>0.98250000000000004</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="65">
         <v>0.97119999999999995</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="65">
         <v>0.94359999999999999</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="66">
         <v>0.83579999999999999</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="64">
         <f t="shared" si="5"/>
         <v>0.93327499999999997</v>
       </c>
       <c r="G18" s="45"/>
-      <c r="H18" s="25">
+      <c r="H18" s="63">
         <v>0.98309999999999997</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="65">
         <v>0.97430000000000005</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="65">
         <v>0.9476</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="66">
         <v>0.90539999999999998</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="11">
         <f>AVERAGE(H18:K18)</f>
         <v>0.95260000000000011</v>
       </c>
-      <c r="N18" s="35">
+      <c r="N18" s="55">
         <v>1</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="56">
         <v>1</v>
       </c>
-      <c r="P18" s="36">
+      <c r="P18" s="57">
         <v>0.97219999999999995</v>
       </c>
-      <c r="Q18" s="8">
+      <c r="Q18" s="11">
         <f t="shared" si="6"/>
         <v>0.99073333333333335</v>
       </c>
       <c r="R18" s="8"/>
-      <c r="S18" s="35">
+      <c r="S18" s="55">
         <v>0.99019999999999997</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="56">
         <v>1</v>
       </c>
-      <c r="U18" s="36">
+      <c r="U18" s="57">
         <v>1</v>
       </c>
-      <c r="V18" s="8">
+      <c r="V18" s="11">
         <f t="shared" si="7"/>
         <v>0.99673333333333325</v>
       </c>

</xml_diff>